<commit_message>
added Add New Client feature
</commit_message>
<xml_diff>
--- a/P1-Rosa/P1-Reports.xlsx
+++ b/P1-Rosa/P1-Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature\Gallaway_A-P1\P1-Rosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30F568D-F6B7-48B6-AC88-0824F8F7B5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7079C9B-90E5-40E8-819B-D8B92225E00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>firstName</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Zip Code</t>
   </si>
   <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
     <t>Customer ID</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t>Alice.Appleton@gallaway.us</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Bob</t>
   </si>
   <si>
@@ -113,6 +119,27 @@
   </si>
   <si>
     <t>Frank.Scratch@gallaway.us</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Gallaway</t>
+  </si>
+  <si>
+    <t>aaron@gallaway.us</t>
+  </si>
+  <si>
+    <t>401-378-6008</t>
+  </si>
+  <si>
+    <t>52 valley street</t>
+  </si>
+  <si>
+    <t>providence</t>
+  </si>
+  <si>
+    <t>ri</t>
   </si>
 </sst>
 </file>
@@ -477,16 +504,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,71 +537,211 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1">
+        <v>814535</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1">
+        <v>733079</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1">
+        <v>748804</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1">
+        <v>861710</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1">
+        <v>181511</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1">
+        <v>165856</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8">
+        <v>2909</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8">
+        <v>931741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Add Order feature
</commit_message>
<xml_diff>
--- a/P1-Rosa/P1-Reports.xlsx
+++ b/P1-Rosa/P1-Reports.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature\Gallaway_A-P1\P1-Rosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D155E068-FCBC-4023-8A8F-F1638BDA67E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1584848E-842F-4670-99E3-5A10A8DC3F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
+    <workbookView xWindow="5460" yWindow="1164" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Client List" sheetId="4" r:id="rId2"/>
+    <sheet name="Orders" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>firstName</t>
   </si>
@@ -143,6 +144,21 @@
   </si>
   <si>
     <t>02909</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>yacht club soda</t>
+  </si>
+  <si>
+    <t>quohogs</t>
   </si>
 </sst>
 </file>
@@ -511,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -523,6 +539,7 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="3"/>
     <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -761,4 +778,65 @@
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C84F606-4304-4F84-B841-8E47F318DC6D}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>706167</v>
+      </c>
+      <c r="D2">
+        <v>66146698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>706167</v>
+      </c>
+      <c r="D3">
+        <v>93349827</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pulled data from vendor sites, changes to add client & add shopping list
</commit_message>
<xml_diff>
--- a/P1-Rosa/P1-Reports.xlsx
+++ b/P1-Rosa/P1-Reports.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature\Gallaway_A-P1\P1-Rosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1584848E-842F-4670-99E3-5A10A8DC3F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A886C8-D8D0-417C-9FEE-65017C3EB3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="1164" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
+    <workbookView xWindow="-12315" yWindow="-9645" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Client List" sheetId="4" r:id="rId2"/>
-    <sheet name="Orders" sheetId="5" r:id="rId3"/>
+    <sheet name="Products" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>firstName</t>
   </si>
@@ -47,21 +47,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
     <t>Customer ID</t>
   </si>
   <si>
@@ -74,9 +59,6 @@
     <t>Alice.Appleton@gallaway.us</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Bob</t>
   </si>
   <si>
@@ -122,51 +104,204 @@
     <t>Frank.Scratch@gallaway.us</t>
   </si>
   <si>
+    <t>Item</t>
+  </si>
+  <si>
     <t>Aaron</t>
   </si>
   <si>
     <t>Gallaway</t>
   </si>
   <si>
-    <t>aaron@gallaway.us</t>
-  </si>
-  <si>
-    <t>52 Valley Street</t>
-  </si>
-  <si>
-    <t>RI</t>
-  </si>
-  <si>
-    <t>401-378-6008</t>
-  </si>
-  <si>
-    <t>Providence</t>
-  </si>
-  <si>
-    <t>02909</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Order ID</t>
-  </si>
-  <si>
-    <t>yacht club soda</t>
-  </si>
-  <si>
-    <t>quohogs</t>
+    <t>aaron.gallaway@revature.net</t>
+  </si>
+  <si>
+    <t>Coffe Milk</t>
+  </si>
+  <si>
+    <t>Yacht Club Soda</t>
+  </si>
+  <si>
+    <t>Quohogs</t>
+  </si>
+  <si>
+    <t>Wicked Big RI Kit</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Chang</t>
+  </si>
+  <si>
+    <t>Chartreuse verte</t>
+  </si>
+  <si>
+    <t>Cote de Blaye</t>
+  </si>
+  <si>
+    <t>Guarana Fantastica</t>
+  </si>
+  <si>
+    <t>Ipoh Coffee</t>
+  </si>
+  <si>
+    <t>Lakkalikoori</t>
+  </si>
+  <si>
+    <t>Laughing Lumberjack Lager</t>
+  </si>
+  <si>
+    <t>Outback Lager</t>
+  </si>
+  <si>
+    <t>Rhonbrau Klosterbier</t>
+  </si>
+  <si>
+    <t>Sasquatch Ale</t>
+  </si>
+  <si>
+    <t>Steeleye Stout</t>
+  </si>
+  <si>
+    <t>Chai  (open in a new window)</t>
+  </si>
+  <si>
+    <t>Aniseed Syrup</t>
+  </si>
+  <si>
+    <t>Chef Anton's Cajun Seasoning</t>
+  </si>
+  <si>
+    <t>Chef Anton's Gumbo Mix</t>
+  </si>
+  <si>
+    <t>Genen Shouyu</t>
+  </si>
+  <si>
+    <t>Grandma's Boysenberry Spread</t>
+  </si>
+  <si>
+    <t>Gula Malacca</t>
+  </si>
+  <si>
+    <t>Louisiana Fiery Hot Pepper Sauce</t>
+  </si>
+  <si>
+    <t>Louisiana Hot Spiced Okra</t>
+  </si>
+  <si>
+    <t>Northwoods Cranberry Sauce</t>
+  </si>
+  <si>
+    <t>Original Frankfurter Grune SoBe</t>
+  </si>
+  <si>
+    <t>Sirop d'erable</t>
+  </si>
+  <si>
+    <t>Veggie Spread</t>
+  </si>
+  <si>
+    <t>LR64001850</t>
+  </si>
+  <si>
+    <t>LR44275402</t>
+  </si>
+  <si>
+    <t>LR73132699</t>
+  </si>
+  <si>
+    <t>LR79415701</t>
+  </si>
+  <si>
+    <t>PB22182282</t>
+  </si>
+  <si>
+    <t>PB38183442</t>
+  </si>
+  <si>
+    <t>PB12173992</t>
+  </si>
+  <si>
+    <t>PB95600857</t>
+  </si>
+  <si>
+    <t>PB96876192</t>
+  </si>
+  <si>
+    <t>PB13159195</t>
+  </si>
+  <si>
+    <t>PB41719313</t>
+  </si>
+  <si>
+    <t>PB27297711</t>
+  </si>
+  <si>
+    <t>PB60865497</t>
+  </si>
+  <si>
+    <t>PB52422674</t>
+  </si>
+  <si>
+    <t>PB13557087</t>
+  </si>
+  <si>
+    <t>PB39276405</t>
+  </si>
+  <si>
+    <t>PS95809333</t>
+  </si>
+  <si>
+    <t>PS40949632</t>
+  </si>
+  <si>
+    <t>PS26230852</t>
+  </si>
+  <si>
+    <t>PS46645325</t>
+  </si>
+  <si>
+    <t>PS59211329</t>
+  </si>
+  <si>
+    <t>PS29766723</t>
+  </si>
+  <si>
+    <t>PS10040275</t>
+  </si>
+  <si>
+    <t>PS85321494</t>
+  </si>
+  <si>
+    <t>PS46158730</t>
+  </si>
+  <si>
+    <t>PS73450560</t>
+  </si>
+  <si>
+    <t>PS13583192</t>
+  </si>
+  <si>
+    <t>PS16431038</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -194,11 +329,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,250 +665,137 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="3"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1">
-        <v>814535</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>196268</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1">
-        <v>733079</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
+        <v>566297</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="1">
-        <v>748804</v>
+      <c r="D4" s="1">
+        <v>964734</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1">
-        <v>861710</v>
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>356280</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1">
-        <v>181511</v>
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>851898</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>594776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1">
-        <v>165856</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8">
-        <v>706167</v>
+      <c r="D8" s="1">
+        <v>705353</v>
       </c>
     </row>
   </sheetData>
@@ -782,58 +806,246 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C84F606-4304-4F84-B841-8E47F318DC6D}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B14" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>706167</v>
-      </c>
-      <c r="D2">
-        <v>66146698</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>706167</v>
-      </c>
-      <c r="D3">
-        <v>93349827</v>
+      <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created DB for clients
</commit_message>
<xml_diff>
--- a/P1-Rosa/P1-Reports.xlsx
+++ b/P1-Rosa/P1-Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature\Gallaway_A-P1\P1-Rosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A886C8-D8D0-417C-9FEE-65017C3EB3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFD6D6A-788C-4BDF-A1B0-9816911780FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12315" yWindow="-9645" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
+    <workbookView xWindow="3708" yWindow="1692" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,184 +107,184 @@
     <t>Item</t>
   </si>
   <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Coffe Milk</t>
+  </si>
+  <si>
+    <t>LR64001850</t>
+  </si>
+  <si>
+    <t>Yacht Club Soda</t>
+  </si>
+  <si>
+    <t>LR44275402</t>
+  </si>
+  <si>
+    <t>Quohogs</t>
+  </si>
+  <si>
+    <t>LR73132699</t>
+  </si>
+  <si>
+    <t>Wicked Big RI Kit</t>
+  </si>
+  <si>
+    <t>LR79415701</t>
+  </si>
+  <si>
+    <t>Chai  (open in a new window)</t>
+  </si>
+  <si>
+    <t>PB22182282</t>
+  </si>
+  <si>
+    <t>Chang</t>
+  </si>
+  <si>
+    <t>PB38183442</t>
+  </si>
+  <si>
+    <t>Chartreuse verte</t>
+  </si>
+  <si>
+    <t>PB12173992</t>
+  </si>
+  <si>
+    <t>Cote de Blaye</t>
+  </si>
+  <si>
+    <t>PB95600857</t>
+  </si>
+  <si>
+    <t>Guarana Fantastica</t>
+  </si>
+  <si>
+    <t>PB96876192</t>
+  </si>
+  <si>
+    <t>Ipoh Coffee</t>
+  </si>
+  <si>
+    <t>PB13159195</t>
+  </si>
+  <si>
+    <t>Lakkalikoori</t>
+  </si>
+  <si>
+    <t>PB41719313</t>
+  </si>
+  <si>
+    <t>Laughing Lumberjack Lager</t>
+  </si>
+  <si>
+    <t>PB27297711</t>
+  </si>
+  <si>
+    <t>Outback Lager</t>
+  </si>
+  <si>
+    <t>PB60865497</t>
+  </si>
+  <si>
+    <t>Rhonbrau Klosterbier</t>
+  </si>
+  <si>
+    <t>PB52422674</t>
+  </si>
+  <si>
+    <t>Sasquatch Ale</t>
+  </si>
+  <si>
+    <t>PB13557087</t>
+  </si>
+  <si>
+    <t>Steeleye Stout</t>
+  </si>
+  <si>
+    <t>PB39276405</t>
+  </si>
+  <si>
+    <t>Aniseed Syrup</t>
+  </si>
+  <si>
+    <t>PS95809333</t>
+  </si>
+  <si>
+    <t>Chef Anton's Cajun Seasoning</t>
+  </si>
+  <si>
+    <t>PS40949632</t>
+  </si>
+  <si>
+    <t>Chef Anton's Gumbo Mix</t>
+  </si>
+  <si>
+    <t>PS26230852</t>
+  </si>
+  <si>
+    <t>Genen Shouyu</t>
+  </si>
+  <si>
+    <t>PS46645325</t>
+  </si>
+  <si>
+    <t>Grandma's Boysenberry Spread</t>
+  </si>
+  <si>
+    <t>PS59211329</t>
+  </si>
+  <si>
+    <t>Gula Malacca</t>
+  </si>
+  <si>
+    <t>PS29766723</t>
+  </si>
+  <si>
+    <t>Louisiana Fiery Hot Pepper Sauce</t>
+  </si>
+  <si>
+    <t>PS10040275</t>
+  </si>
+  <si>
+    <t>Louisiana Hot Spiced Okra</t>
+  </si>
+  <si>
+    <t>PS85321494</t>
+  </si>
+  <si>
+    <t>Northwoods Cranberry Sauce</t>
+  </si>
+  <si>
+    <t>PS46158730</t>
+  </si>
+  <si>
+    <t>Original Frankfurter Grune SoBe</t>
+  </si>
+  <si>
+    <t>PS73450560</t>
+  </si>
+  <si>
+    <t>Sirop d'erable</t>
+  </si>
+  <si>
+    <t>PS13583192</t>
+  </si>
+  <si>
+    <t>Veggie Spread</t>
+  </si>
+  <si>
+    <t>PS16431038</t>
+  </si>
+  <si>
     <t>Aaron</t>
   </si>
   <si>
     <t>Gallaway</t>
   </si>
   <si>
-    <t>aaron.gallaway@revature.net</t>
-  </si>
-  <si>
-    <t>Coffe Milk</t>
-  </si>
-  <si>
-    <t>Yacht Club Soda</t>
-  </si>
-  <si>
-    <t>Quohogs</t>
-  </si>
-  <si>
-    <t>Wicked Big RI Kit</t>
-  </si>
-  <si>
-    <t>Product ID</t>
-  </si>
-  <si>
-    <t>Chang</t>
-  </si>
-  <si>
-    <t>Chartreuse verte</t>
-  </si>
-  <si>
-    <t>Cote de Blaye</t>
-  </si>
-  <si>
-    <t>Guarana Fantastica</t>
-  </si>
-  <si>
-    <t>Ipoh Coffee</t>
-  </si>
-  <si>
-    <t>Lakkalikoori</t>
-  </si>
-  <si>
-    <t>Laughing Lumberjack Lager</t>
-  </si>
-  <si>
-    <t>Outback Lager</t>
-  </si>
-  <si>
-    <t>Rhonbrau Klosterbier</t>
-  </si>
-  <si>
-    <t>Sasquatch Ale</t>
-  </si>
-  <si>
-    <t>Steeleye Stout</t>
-  </si>
-  <si>
-    <t>Chai  (open in a new window)</t>
-  </si>
-  <si>
-    <t>Aniseed Syrup</t>
-  </si>
-  <si>
-    <t>Chef Anton's Cajun Seasoning</t>
-  </si>
-  <si>
-    <t>Chef Anton's Gumbo Mix</t>
-  </si>
-  <si>
-    <t>Genen Shouyu</t>
-  </si>
-  <si>
-    <t>Grandma's Boysenberry Spread</t>
-  </si>
-  <si>
-    <t>Gula Malacca</t>
-  </si>
-  <si>
-    <t>Louisiana Fiery Hot Pepper Sauce</t>
-  </si>
-  <si>
-    <t>Louisiana Hot Spiced Okra</t>
-  </si>
-  <si>
-    <t>Northwoods Cranberry Sauce</t>
-  </si>
-  <si>
-    <t>Original Frankfurter Grune SoBe</t>
-  </si>
-  <si>
-    <t>Sirop d'erable</t>
-  </si>
-  <si>
-    <t>Veggie Spread</t>
-  </si>
-  <si>
-    <t>LR64001850</t>
-  </si>
-  <si>
-    <t>LR44275402</t>
-  </si>
-  <si>
-    <t>LR73132699</t>
-  </si>
-  <si>
-    <t>LR79415701</t>
-  </si>
-  <si>
-    <t>PB22182282</t>
-  </si>
-  <si>
-    <t>PB38183442</t>
-  </si>
-  <si>
-    <t>PB12173992</t>
-  </si>
-  <si>
-    <t>PB95600857</t>
-  </si>
-  <si>
-    <t>PB96876192</t>
-  </si>
-  <si>
-    <t>PB13159195</t>
-  </si>
-  <si>
-    <t>PB41719313</t>
-  </si>
-  <si>
-    <t>PB27297711</t>
-  </si>
-  <si>
-    <t>PB60865497</t>
-  </si>
-  <si>
-    <t>PB52422674</t>
-  </si>
-  <si>
-    <t>PB13557087</t>
-  </si>
-  <si>
-    <t>PB39276405</t>
-  </si>
-  <si>
-    <t>PS95809333</t>
-  </si>
-  <si>
-    <t>PS40949632</t>
-  </si>
-  <si>
-    <t>PS26230852</t>
-  </si>
-  <si>
-    <t>PS46645325</t>
-  </si>
-  <si>
-    <t>PS59211329</t>
-  </si>
-  <si>
-    <t>PS29766723</t>
-  </si>
-  <si>
-    <t>PS10040275</t>
-  </si>
-  <si>
-    <t>PS85321494</t>
-  </si>
-  <si>
-    <t>PS46158730</t>
-  </si>
-  <si>
-    <t>PS73450560</t>
-  </si>
-  <si>
-    <t>PS13583192</t>
-  </si>
-  <si>
-    <t>PS16431038</t>
+    <t>aaron@gallaway.us</t>
   </si>
 </sst>
 </file>
@@ -329,13 +329,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,9 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -676,31 +673,27 @@
     <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="4" customWidth="1"/>
     <col min="8" max="8" width="13.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,10 +704,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="1">
-        <v>196268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>809935</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -725,10 +718,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="1">
-        <v>566297</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>505708</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -739,10 +732,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="1">
-        <v>964734</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>377146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -753,10 +746,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="1">
-        <v>356280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>747175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -767,10 +760,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="1">
-        <v>851898</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>471356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -781,21 +774,21 @@
         <v>21</v>
       </c>
       <c r="D7" s="1">
-        <v>594776</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>615642</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1">
-        <v>705353</v>
+        <v>127508</v>
       </c>
     </row>
   </sheetData>
@@ -808,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C84F606-4304-4F84-B841-8E47F318DC6D}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -816,28 +809,28 @@
     <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -845,207 +838,207 @@
         <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor update to website and added DB for shopping list
</commit_message>
<xml_diff>
--- a/P1-Rosa/P1-Reports.xlsx
+++ b/P1-Rosa/P1-Reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature\Gallaway_A-P1\P1-Rosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A1B9D9-3BAC-4A74-93E8-B867E65F07B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696E4527-2CC5-47D1-8389-1504E66DE84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3708" yWindow="1692" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
   <si>
     <t>firstName</t>
   </si>
@@ -288,16 +288,22 @@
     <t>aaron@gallaway.us</t>
   </si>
   <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Client ID</t>
+  </si>
+  <si>
+    <t>List ID</t>
+  </si>
+  <si>
     <t>Coffee Milk</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Client ID</t>
-  </si>
-  <si>
-    <t>List ID</t>
+    <t>Yacht Soda</t>
+  </si>
+  <si>
+    <t>beer</t>
   </si>
 </sst>
 </file>
@@ -675,9 +681,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB6D459-5F93-4B5C-8864-69CCAF9459BD}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -689,27 +697,27 @@
         <v>22</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>127508</v>
       </c>
       <c r="D2">
-        <v>41583983</v>
+        <v>68307346</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -717,13 +725,41 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>127508</v>
       </c>
       <c r="D3">
-        <v>13812604</v>
+        <v>19541231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>127508</v>
+      </c>
+      <c r="D4">
+        <v>88747923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>127508</v>
+      </c>
+      <c r="D5">
+        <v>12345678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a working version of buy from pega
</commit_message>
<xml_diff>
--- a/P1-Rosa/P1-Reports.xlsx
+++ b/P1-Rosa/P1-Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature\Gallaway_A-P1\P1-Rosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696E4527-2CC5-47D1-8389-1504E66DE84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09206C26-E383-49B8-A347-9A5198B4B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3708" yWindow="1692" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
   <si>
     <t>firstName</t>
   </si>
@@ -303,7 +303,7 @@
     <t>Yacht Soda</t>
   </si>
   <si>
-    <t>beer</t>
+    <t>Chai</t>
   </si>
 </sst>
 </file>
@@ -681,10 +681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB6D459-5F93-4B5C-8864-69CCAF9459BD}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,16 +750,58 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>127508</v>
       </c>
       <c r="D5">
-        <v>12345678</v>
+        <v>47414620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>127508</v>
+      </c>
+      <c r="D6">
+        <v>37614806</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>127508</v>
+      </c>
+      <c r="D7">
+        <v>73752320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>127508</v>
+      </c>
+      <c r="D8">
+        <v>36295933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added buy many items from pega feature
</commit_message>
<xml_diff>
--- a/P1-Rosa/P1-Reports.xlsx
+++ b/P1-Rosa/P1-Reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature\Gallaway_A-P1\P1-Rosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09206C26-E383-49B8-A347-9A5198B4B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB22191-FF7B-4116-BD0B-8D5835B3DEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{AB2E9848-6D37-4C9C-B68D-C5DFA84EDA92}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>firstName</t>
   </si>
@@ -295,15 +295,6 @@
   </si>
   <si>
     <t>List ID</t>
-  </si>
-  <si>
-    <t>Coffee Milk</t>
-  </si>
-  <si>
-    <t>Yacht Soda</t>
-  </si>
-  <si>
-    <t>Chai</t>
   </si>
 </sst>
 </file>
@@ -681,7 +672,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB6D459-5F93-4B5C-8864-69CCAF9459BD}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -689,7 +680,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -708,100 +699,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>127508</v>
       </c>
       <c r="D2">
-        <v>68307346</v>
+        <v>47414620</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>127508</v>
       </c>
       <c r="D3">
-        <v>19541231</v>
+        <v>37614806</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>127508</v>
       </c>
       <c r="D4">
-        <v>88747923</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>127508</v>
-      </c>
-      <c r="D5">
-        <v>47414620</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>127508</v>
-      </c>
-      <c r="D6">
-        <v>37614806</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>127508</v>
-      </c>
-      <c r="D7">
-        <v>73752320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>127508</v>
-      </c>
-      <c r="D8">
-        <v>36295933</v>
+        <v>12345678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>